<commit_message>
Update ATD03b Beregn Bruttofortjeneste.xlsx
2. udgave af ATD03b Beregn Bruttofortjeneste
Coauthors: Nikolaj
Reviewers: Mik

Co-Authored-By: Nikolaj Thor Christensen <nikothor@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/05 Test/ATD03b Beregn Bruttofortjeneste.xlsx
+++ b/05 Test/ATD03b Beregn Bruttofortjeneste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alter\Documents\GitHub\HoeKulator\05 Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3B3E071-9D93-41D3-90C4-8F90227924EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27510C65-ECF2-4699-ACA3-AD023A42B0CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E96B9F9D-9139-4AC8-8EC5-3427FAD41271}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Vareforbrug = 200</t>
   </si>
   <si>
-    <t>Bruttofortjeneste = -100</t>
-  </si>
-  <si>
     <t>Omsætning = A</t>
   </si>
   <si>
@@ -65,22 +62,82 @@
     <t>Fejl forkertDatatype Vareforbrug = A</t>
   </si>
   <si>
-    <t>Fejl forkertDatatype Omsætning = A, Vareforbrug = A</t>
-  </si>
-  <si>
-    <t>Omsætning = -100</t>
-  </si>
-  <si>
-    <t>Vareforbrug = -100</t>
-  </si>
-  <si>
-    <t>Fejl negativtBeløb Omsætning = -100, Vareforbrug = -100</t>
+    <t>Tester om resultat/formlen passer</t>
+  </si>
+  <si>
+    <t>Omsætning = 100,00</t>
+  </si>
+  <si>
+    <t>Tester om resultat er String</t>
+  </si>
+  <si>
+    <t>Omsætning = brutto</t>
+  </si>
+  <si>
+    <t>Fejl forkertDatatype Omsætning = brutto</t>
+  </si>
+  <si>
+    <t>Omsætning = 200</t>
+  </si>
+  <si>
+    <t>Vareforbrug = brutto</t>
+  </si>
+  <si>
+    <t>Fejl forkertDatatype Vareforbrug = brutto</t>
+  </si>
+  <si>
+    <t>Vareforbrug = 50,25</t>
+  </si>
+  <si>
+    <t>Bruttofortjeneste</t>
+  </si>
+  <si>
+    <t>49,75</t>
+  </si>
+  <si>
+    <t>Beskrivelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruttofortjeneste </t>
+  </si>
+  <si>
+    <t>Tester om resultat er Char</t>
+  </si>
+  <si>
+    <t>Omsætning = 100,25</t>
+  </si>
+  <si>
+    <t>Vareforbrug = 50</t>
+  </si>
+  <si>
+    <t>Vareforbrug = 50,456</t>
+  </si>
+  <si>
+    <t>Omsætning = 100,456</t>
+  </si>
+  <si>
+    <t>vareforbrug = 50</t>
+  </si>
+  <si>
+    <t>49,54</t>
+  </si>
+  <si>
+    <t>50,25</t>
+  </si>
+  <si>
+    <t>50,46</t>
+  </si>
+  <si>
+    <t>Tester om resultat regner til rigtigt decimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -197,19 +254,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,108 +631,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298B0673-BFA3-4EB2-B56D-7E26469A092E}">
-  <dimension ref="A4:C14"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+      <c r="D4" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12">
+        <v>100</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="7"/>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>